<commit_message>
fiksin vse chto toka moznka
</commit_message>
<xml_diff>
--- a/File/MatLab/2/LBD.xlsx
+++ b/File/MatLab/2/LBD.xlsx
@@ -319,452 +319,752 @@
   <sheetData>
     <row r="1">
       <c r="A1">
-        <v>49.2192553663315</v>
+        <v>73.65148208090005</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>46.66499496130486</v>
+        <v>71.5654190831555</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>6.425057258033563</v>
+        <v>12.15103083423297</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>6.225622390795331</v>
+        <v>11.426392493482673</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4.37249974377782</v>
+        <v>6.3657058416708665</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>4.01763136678266</v>
+        <v>6.2668354387146215</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>3.988470187946177</v>
+        <v>6.018524849238329</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>3.8265237840041384</v>
+        <v>5.649278881567422</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>3.0308177376527423</v>
+        <v>4.894450650526875</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>3.0141573409113804</v>
+        <v>4.846680506968446</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>2.168783086622889</v>
+        <v>3.3180148797316704</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>2.164565770990723</v>
+        <v>3.1468888293667807</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>1.8542786348992464</v>
+        <v>2.9178419344113253</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>1.8304105952788943</v>
+        <v>2.8721289066602838</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>1.7899937787377715</v>
+        <v>2.670463918754725</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>1.7401771032887647</v>
+        <v>2.630459087462568</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>1.3164208781860034</v>
+        <v>2.2475412465946856</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>1.2897413446131323</v>
+        <v>2.144898641005488</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>1.2353964931997028</v>
+        <v>1.9074099873174817</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>1.1150913187606404</v>
+        <v>1.8695986000392686</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>0.763034127217647</v>
+        <v>1.6913328205314564</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>0.5490584089418387</v>
+        <v>1.5945974269300172</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>0.30335490936695575</v>
+        <v>1.3933967291190794</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>0.2269064650125829</v>
+        <v>1.3856417119495559</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>0.10808378379901519</v>
+        <v>1.356421292285049</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>0.06980034744334342</v>
+        <v>1.3353592588978371</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>0.04718977102802561</v>
+        <v>1.3134652563017128</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>0.04359600135651035</v>
+        <v>1.3050398746224352</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>0.019455030031951277</v>
+        <v>1.2230034804802028</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>0.01178988045373338</v>
+        <v>1.2184526866887373</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>0.011537107228336651</v>
+        <v>1.1370577909168755</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>0.009034274882051843</v>
+        <v>1.1166461095520606</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>0.006225726966626838</v>
+        <v>0.9126170840170339</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>0.005728135502780364</v>
+        <v>0.7573962970162427</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>0.005059238598815126</v>
+        <v>0.5061659406008099</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>0.00392207219654244</v>
+        <v>0.44811322979533025</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>0.0035816867273676333</v>
+        <v>0.299233302410026</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>0.0034409516866128363</v>
+        <v>0.23882809096418925</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>0.003102151467620049</v>
+        <v>0.14763480396613896</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>0.0030327836476259176</v>
+        <v>0.10690207544706783</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>0.0026552908583552443</v>
+        <v>0.08066015286641881</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>0.002424890042542299</v>
+        <v>0.06117751155458824</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>0.0023080852005950394</v>
+        <v>0.0516237354924994</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>0.002156459635052557</v>
+        <v>0.039216235553200175</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>0.0020600437098013758</v>
+        <v>0.033924354672567075</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>0.0019503781807711305</v>
+        <v>0.02818353484368433</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>0.0019161145997699967</v>
+        <v>0.018706762401778276</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>0.0017741984541524607</v>
+        <v>0.01606118750660833</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>0.001695203599623755</v>
+        <v>0.01536831940283495</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>0.001623519422586601</v>
+        <v>0.009854138697556534</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>0.0015881823764141766</v>
+        <v>0.0090437283024589</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>0.001569529132016839</v>
+        <v>0.008995381662573887</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>0.0015407825894260007</v>
+        <v>0.006607137195720241</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>0.0015368852971244982</v>
+        <v>0.0056186561312976425</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>0.001240582264107951</v>
+        <v>0.005459864843209241</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>0.001234629424613124</v>
+        <v>0.00467372986271009</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>0.00120696677766793</v>
+        <v>0.004147896918771631</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>0.001045760059012165</v>
+        <v>0.0038359442959082692</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>0.000982226769331781</v>
+        <v>0.003657711172858614</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>0.0009514934059664235</v>
+        <v>0.003455151786063285</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>0.0008906942513391133</v>
+        <v>0.003385924633234284</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>0.0008314084154736878</v>
+        <v>0.0032070780191149647</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>0.0007947040864288039</v>
+        <v>0.003076779081074718</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>0.0007913892203593144</v>
+        <v>0.0030534422443745856</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>0.0007860634318852944</v>
+        <v>0.0027970848477307116</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>0.0007793398741407497</v>
+        <v>0.002717332598026908</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>0.000760463821155674</v>
+        <v>0.002699221848845295</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>0.0007524823958461217</v>
+        <v>0.0025683882405719847</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>0.0007382940174242309</v>
+        <v>0.0024886911039145596</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>0.0007189296121127635</v>
+        <v>0.0023960851416382324</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>0.000703808766389829</v>
+        <v>0.0023680908144621668</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>0.0006853118291148197</v>
+        <v>0.0023045919865055924</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>0.0006607968766783136</v>
+        <v>0.0020452421299154743</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>0.0006579575205094721</v>
+        <v>0.0020069690815275555</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>0.0006406210379804969</v>
+        <v>0.002006822961407528</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>0.0006192181544406505</v>
+        <v>0.0019843201841516995</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>0.000599901010086995</v>
+        <v>0.001966889910796623</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>0.0005837380262720801</v>
+        <v>0.0018018616106045399</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>0.0005642317068990036</v>
+        <v>0.0017809898157123698</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>0.0005149446529393639</v>
+        <v>0.0017736190299969129</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>0.0005063988372739562</v>
+        <v>0.001662841246094959</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>0.00048434415268644644</v>
+        <v>0.0015985812173693512</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>0.00047278330533921675</v>
+        <v>0.0015582334425136564</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>0.00046934086485511163</v>
+        <v>0.0015268716892666548</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>0.0004103919832242806</v>
+        <v>0.001469457763706943</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>0.0003830599284686883</v>
+        <v>0.001467536430491016</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>0.00037598935942710285</v>
+        <v>0.0014037750422028802</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>0.0003557382626954658</v>
+        <v>0.0012506835340837775</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>0.00027387189036013633</v>
+        <v>0.0012367690572032172</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>0.0002634813764464955</v>
+        <v>0.0012241624914952744</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>0.001204129189837505</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>0.0011471813705538677</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>0.0011395248216345575</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>0.0011357566921070962</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>0.0010977174281391901</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>0.0010866867461262063</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>0.0010806234782664691</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>0.0010405661219855275</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>0.0009966494655046908</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>0.0009949099246063606</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>0.0009787861796821961</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
+        <v>0.000977803518505653</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103">
+        <v>0.0009743933140480024</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>0.0009732708801080717</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105">
+        <v>0.000940511097573523</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>0.0009118514251224665</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107">
+        <v>0.0008744708249892553</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108">
+        <v>0.0008526734599615674</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109">
+        <v>0.0008219158188079482</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <v>0.0007878001323665303</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111">
+        <v>0.0007728887291290534</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112">
+        <v>0.0007689752150222075</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113">
+        <v>0.0007518125389021705</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114">
+        <v>0.0007377389184933806</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115">
+        <v>0.0007167198878757198</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116">
+        <v>0.0007050346412913177</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117">
+        <v>0.000703134373748179</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118">
+        <v>0.0006810349004230626</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119">
+        <v>0.0006778373291260104</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120">
+        <v>0.0006548477777994086</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121">
+        <v>0.0006508711227124996</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122">
+        <v>0.0006486590664545881</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123">
+        <v>0.0006483967356305447</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124">
+        <v>0.0006406891664693552</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125">
+        <v>0.0006363472058167124</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126">
+        <v>0.0006082172221525704</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127">
+        <v>0.0006069996074795361</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128">
+        <v>0.0005804914076622242</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129">
+        <v>0.0005781974380133214</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130">
+        <v>0.0005391348426972122</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131">
+        <v>0.0004824044080269323</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132">
+        <v>0.0004797384102598265</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133">
+        <v>0.00046712699296051036</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134">
+        <v>0.00045795791303395193</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135">
+        <v>0.00045181829095976083</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136">
+        <v>0.00045103939804816477</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137">
+        <v>0.0004445405538737733</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138">
+        <v>0.00041448600340059186</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139">
+        <v>0.0004128167317757558</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140">
+        <v>0.00040628564781553206</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141">
+        <v>0.00040309505131717335</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142">
+        <v>0.0003980364371124916</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143">
+        <v>0.0003509577396593601</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144">
+        <v>0.0003280882994556986</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145">
+        <v>0.0003076011747652274</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146">
+        <v>0.0003039851943664237</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147">
+        <v>0.000290357114979041</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148">
+        <v>0.0002862857134435256</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149">
+        <v>0.00022244058040534642</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150">
+        <v>0.00021445972501369243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>